<commit_message>
changed diet storage format
</commit_message>
<xml_diff>
--- a/artificial_pancreas/db/diets/highBGL.xlsx
+++ b/artificial_pancreas/db/diets/highBGL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brooklyn/Documents/GITHUB/APS/APS/artificial_pancreas/db/diets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\APS\artificial_pancreas\db\diets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DE0B83-D87E-4648-94AD-C8D8696B367F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CD9987-DAD4-4078-A422-4356420B7EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15360" xr2:uid="{4B5383E1-92E3-4F49-82E4-F541FD6A9B93}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="23040" windowHeight="12120" xr2:uid="{4B5383E1-92E3-4F49-82E4-F541FD6A9B93}"/>
   </bookViews>
   <sheets>
     <sheet name="DIET student 3" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Day</t>
   </si>
@@ -64,24 +64,6 @@
   </si>
   <si>
     <t>INSULIN</t>
-  </si>
-  <si>
-    <t>AVG</t>
-  </si>
-  <si>
-    <t>SD</t>
-  </si>
-  <si>
-    <t>GMI</t>
-  </si>
-  <si>
-    <t>TIR_HIGH</t>
-  </si>
-  <si>
-    <t>TIR_IN_RANGE</t>
-  </si>
-  <si>
-    <t>TIR_LOW</t>
   </si>
 </sst>
 </file>
@@ -133,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -142,6 +124,7 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,30 +442,30 @@
   <dimension ref="A1:M290"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="6"/>
-    <col min="2" max="2" width="11.83203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" style="6"/>
+    <col min="2" max="2" width="11.796875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="15.296875" style="6" customWidth="1"/>
     <col min="4" max="4" width="24" style="6" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="29.83203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="6"/>
-    <col min="8" max="8" width="16.33203125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="30.33203125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="21.83203125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="24.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="22.796875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="29.796875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.796875" style="6"/>
+    <col min="8" max="8" width="16.296875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="18.69921875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="15.69921875" style="6" customWidth="1"/>
+    <col min="11" max="11" width="30.296875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="21.796875" style="6" customWidth="1"/>
+    <col min="13" max="13" width="24.296875" style="6" customWidth="1"/>
     <col min="14" max="14" width="18.5" style="6" customWidth="1"/>
     <col min="15" max="15" width="22" style="6" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="6"/>
+    <col min="16" max="16384" width="10.796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -504,26 +487,14 @@
       <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+    </row>
+    <row r="2" spans="1:13" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -535,7 +506,7 @@
       </c>
       <c r="D2" s="6">
         <f ca="1">RANDBETWEEN(180, 250) + RAND()*(0-0.999)+0.999</f>
-        <v>202.32498110233996</v>
+        <v>222.88714840263688</v>
       </c>
       <c r="E2" s="6">
         <v>0</v>
@@ -546,8 +517,14 @@
       <c r="G2" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -560,11 +537,11 @@
       </c>
       <c r="D3" s="6">
         <f ca="1">RANDBETWEEN(D2-9, D2+9) + RAND()*(-0.999)+0.999</f>
-        <v>209.99543479108655</v>
+        <v>230.9288062776223</v>
       </c>
       <c r="E3" s="6">
         <f ca="1">(D3-D2)/5</f>
-        <v>1.534090737749318</v>
+        <v>1.6083315749970837</v>
       </c>
       <c r="F3" s="6">
         <v>0</v>
@@ -573,7 +550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -586,21 +563,21 @@
       </c>
       <c r="D4" s="6">
         <f t="shared" ref="D4" ca="1" si="1">RANDBETWEEN(D3-9, D3+9) + RAND()*(-0.999)+0.999</f>
-        <v>215.18533247900237</v>
+        <v>228.37809550900462</v>
       </c>
       <c r="E4" s="6">
         <f t="shared" ref="E4" ca="1" si="2">(D4-D3)/5</f>
-        <v>1.0379795375831633</v>
+        <v>-0.51014215372353533</v>
       </c>
       <c r="F4" s="6">
         <f ca="1">(E4-E3)/5</f>
-        <v>-9.9222240033230949E-2</v>
+        <v>-0.42369474574412375</v>
       </c>
       <c r="G4" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -612,7 +589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -624,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -636,7 +613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -648,7 +625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>1</v>
       </c>
@@ -660,7 +637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>1</v>
       </c>
@@ -672,7 +649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>1</v>
       </c>
@@ -684,7 +661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>1</v>
       </c>
@@ -696,7 +673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>1</v>
       </c>
@@ -709,7 +686,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>1</v>
       </c>
@@ -721,7 +698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>1</v>
       </c>
@@ -733,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>1</v>
       </c>
@@ -745,7 +722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>1</v>
       </c>
@@ -757,7 +734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>1</v>
       </c>
@@ -769,7 +746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>1</v>
       </c>
@@ -782,7 +759,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>1</v>
       </c>
@@ -794,7 +771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <v>1</v>
       </c>
@@ -806,7 +783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>1</v>
       </c>
@@ -818,7 +795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
         <v>1</v>
       </c>
@@ -830,7 +807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>1</v>
       </c>
@@ -842,7 +819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <v>1</v>
       </c>
@@ -855,7 +832,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>1</v>
       </c>
@@ -867,7 +844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>1</v>
       </c>
@@ -879,7 +856,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <v>1</v>
       </c>
@@ -891,7 +868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="6">
         <v>1</v>
       </c>
@@ -903,7 +880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
         <v>1</v>
       </c>
@@ -915,7 +892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
         <v>1</v>
       </c>
@@ -927,7 +904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <v>1</v>
       </c>
@@ -939,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>1</v>
       </c>
@@ -951,7 +928,7 @@
         <v>23.07</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="6">
         <v>1</v>
       </c>
@@ -963,7 +940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <v>1</v>
       </c>
@@ -976,7 +953,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="6">
         <v>1</v>
       </c>
@@ -988,7 +965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
         <v>1</v>
       </c>
@@ -1000,7 +977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="6">
         <v>1</v>
       </c>
@@ -1012,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="6">
         <v>1</v>
       </c>
@@ -1024,7 +1001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="6">
         <v>1</v>
       </c>
@@ -1036,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="6">
         <v>1</v>
       </c>
@@ -1048,7 +1025,7 @@
         <v>40.200000000000003</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="6">
         <v>1</v>
       </c>
@@ -1060,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="6">
         <v>1</v>
       </c>
@@ -1072,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="6">
         <v>1</v>
       </c>
@@ -1084,7 +1061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="6">
         <v>1</v>
       </c>
@@ -1096,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
         <v>1</v>
       </c>
@@ -1108,7 +1085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
         <v>1</v>
       </c>
@@ -1120,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="6">
         <v>1</v>
       </c>
@@ -1132,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="6">
         <v>1</v>
       </c>
@@ -1144,7 +1121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
         <v>1</v>
       </c>
@@ -1156,7 +1133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
         <v>1</v>
       </c>
@@ -1168,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="6">
         <v>1</v>
       </c>
@@ -1180,7 +1157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="6">
         <v>1</v>
       </c>
@@ -1192,7 +1169,7 @@
         <v>42.01</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="6">
         <v>1</v>
       </c>
@@ -1204,7 +1181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="6">
         <v>1</v>
       </c>
@@ -1216,7 +1193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
         <v>1</v>
       </c>
@@ -1228,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="6">
         <v>1</v>
       </c>
@@ -1240,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="6">
         <v>1</v>
       </c>
@@ -1252,7 +1229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="6">
         <v>1</v>
       </c>
@@ -1264,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="6">
         <v>1</v>
       </c>
@@ -1276,7 +1253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="6">
         <v>1</v>
       </c>
@@ -1288,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="6">
         <v>1</v>
       </c>
@@ -1300,7 +1277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="6">
         <v>1</v>
       </c>
@@ -1312,7 +1289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="6">
         <v>1</v>
       </c>
@@ -1324,7 +1301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="6">
         <v>1</v>
       </c>
@@ -1336,7 +1313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="6">
         <v>1</v>
       </c>
@@ -1348,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="6">
         <v>1</v>
       </c>
@@ -1360,7 +1337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="6">
         <v>1</v>
       </c>
@@ -1372,7 +1349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="6">
         <v>1</v>
       </c>
@@ -1384,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="6">
         <v>1</v>
       </c>
@@ -1396,7 +1373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="6">
         <v>1</v>
       </c>
@@ -1408,7 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="6">
         <v>1</v>
       </c>
@@ -1420,7 +1397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="6">
         <v>1</v>
       </c>
@@ -1432,7 +1409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="6">
         <v>1</v>
       </c>
@@ -1444,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="6">
         <v>1</v>
       </c>
@@ -1456,7 +1433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="6">
         <v>1</v>
       </c>
@@ -1468,7 +1445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="6">
         <v>1</v>
       </c>
@@ -1480,7 +1457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="6">
         <v>1</v>
       </c>
@@ -1492,7 +1469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="6">
         <v>1</v>
       </c>
@@ -1504,7 +1481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="6">
         <v>1</v>
       </c>
@@ -1516,7 +1493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="6">
         <v>1</v>
       </c>
@@ -1528,7 +1505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="6">
         <v>1</v>
       </c>
@@ -1540,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="6">
         <v>1</v>
       </c>
@@ -1552,7 +1529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="6">
         <v>1</v>
       </c>
@@ -1564,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="6">
         <v>1</v>
       </c>
@@ -1576,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="6">
         <v>1</v>
       </c>
@@ -1588,7 +1565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="6">
         <v>1</v>
       </c>
@@ -1600,7 +1577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="6">
         <v>1</v>
       </c>
@@ -1612,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="6">
         <v>1</v>
       </c>
@@ -1624,7 +1601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="6">
         <v>1</v>
       </c>
@@ -1636,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="6">
         <v>1</v>
       </c>
@@ -1648,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="6">
         <v>1</v>
       </c>
@@ -1660,7 +1637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="6">
         <v>1</v>
       </c>
@@ -1672,7 +1649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="6">
         <v>1</v>
       </c>
@@ -1684,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="6">
         <v>1</v>
       </c>
@@ -1696,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="6">
         <v>1</v>
       </c>
@@ -1708,7 +1685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="6">
         <v>1</v>
       </c>
@@ -1720,7 +1697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="6">
         <v>1</v>
       </c>
@@ -1732,7 +1709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="6">
         <v>1</v>
       </c>
@@ -1744,7 +1721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="6">
         <v>1</v>
       </c>
@@ -1756,7 +1733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="6">
         <v>1</v>
       </c>
@@ -1768,7 +1745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="6">
         <v>1</v>
       </c>
@@ -1780,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="6">
         <v>1</v>
       </c>
@@ -1792,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="6">
         <v>1</v>
       </c>
@@ -1804,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="6">
         <v>1</v>
       </c>
@@ -1816,7 +1793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="6">
         <v>1</v>
       </c>
@@ -1828,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="6">
         <v>1</v>
       </c>
@@ -1840,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="6">
         <v>1</v>
       </c>
@@ -1852,7 +1829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="6">
         <v>1</v>
       </c>
@@ -1864,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="6">
         <v>1</v>
       </c>
@@ -1876,7 +1853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="6">
         <v>1</v>
       </c>
@@ -1888,7 +1865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="6">
         <v>1</v>
       </c>
@@ -1900,7 +1877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="6">
         <v>1</v>
       </c>
@@ -1912,7 +1889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="6">
         <v>1</v>
       </c>
@@ -1924,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="6">
         <v>1</v>
       </c>
@@ -1936,7 +1913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="6">
         <v>1</v>
       </c>
@@ -1948,7 +1925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="6">
         <v>1</v>
       </c>
@@ -1960,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="6">
         <v>1</v>
       </c>
@@ -1972,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="6">
         <v>1</v>
       </c>
@@ -1984,7 +1961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="6">
         <v>1</v>
       </c>
@@ -1996,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="6">
         <v>1</v>
       </c>
@@ -2008,7 +1985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="6">
         <v>1</v>
       </c>
@@ -2020,7 +1997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="6">
         <v>1</v>
       </c>
@@ -2032,7 +2009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="6">
         <v>1</v>
       </c>
@@ -2044,7 +2021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="6">
         <v>1</v>
       </c>
@@ -2056,7 +2033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="6">
         <v>1</v>
       </c>
@@ -2068,7 +2045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="6">
         <v>1</v>
       </c>
@@ -2080,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="6">
         <v>1</v>
       </c>
@@ -2092,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="6">
         <v>1</v>
       </c>
@@ -2104,7 +2081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="6">
         <v>1</v>
       </c>
@@ -2116,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="6">
         <v>1</v>
       </c>
@@ -2128,7 +2105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="6">
         <v>1</v>
       </c>
@@ -2140,7 +2117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="6">
         <v>1</v>
       </c>
@@ -2152,7 +2129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="6">
         <v>1</v>
       </c>
@@ -2164,7 +2141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="6">
         <v>1</v>
       </c>
@@ -2176,7 +2153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="6">
         <v>1</v>
       </c>
@@ -2188,7 +2165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="6">
         <v>1</v>
       </c>
@@ -2200,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="6">
         <v>1</v>
       </c>
@@ -2212,7 +2189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="6">
         <v>1</v>
       </c>
@@ -2224,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" s="6">
         <v>1</v>
       </c>
@@ -2236,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="6">
         <v>1</v>
       </c>
@@ -2248,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="6">
         <v>1</v>
       </c>
@@ -2260,7 +2237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="6">
         <v>1</v>
       </c>
@@ -2272,7 +2249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="6">
         <v>1</v>
       </c>
@@ -2284,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="6">
         <v>1</v>
       </c>
@@ -2296,7 +2273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="6">
         <v>1</v>
       </c>
@@ -2308,7 +2285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" s="6">
         <v>1</v>
       </c>
@@ -2320,7 +2297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="6">
         <v>1</v>
       </c>
@@ -2332,7 +2309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" s="6">
         <v>1</v>
       </c>
@@ -2344,7 +2321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" s="6">
         <v>1</v>
       </c>
@@ -2356,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="6">
         <v>1</v>
       </c>
@@ -2368,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" s="6">
         <v>1</v>
       </c>
@@ -2380,7 +2357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="6">
         <v>1</v>
       </c>
@@ -2392,7 +2369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" s="6">
         <v>1</v>
       </c>
@@ -2404,7 +2381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" s="6">
         <v>1</v>
       </c>
@@ -2416,7 +2393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" s="6">
         <v>1</v>
       </c>
@@ -2428,7 +2405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="6">
         <v>1</v>
       </c>
@@ -2440,7 +2417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" s="6">
         <v>1</v>
       </c>
@@ -2452,7 +2429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" s="6">
         <v>1</v>
       </c>
@@ -2464,7 +2441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" s="6">
         <v>1</v>
       </c>
@@ -2476,7 +2453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="6">
         <v>1</v>
       </c>
@@ -2488,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" s="6">
         <v>1</v>
       </c>
@@ -2500,7 +2477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" s="6">
         <v>1</v>
       </c>
@@ -2512,7 +2489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="6">
         <v>1</v>
       </c>
@@ -2524,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" s="6">
         <v>1</v>
       </c>
@@ -2536,7 +2513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="6">
         <v>1</v>
       </c>
@@ -2548,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" s="6">
         <v>1</v>
       </c>
@@ -2560,7 +2537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="6">
         <v>1</v>
       </c>
@@ -2572,7 +2549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" s="6">
         <v>1</v>
       </c>
@@ -2584,7 +2561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" s="6">
         <v>1</v>
       </c>
@@ -2596,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" s="6">
         <v>1</v>
       </c>
@@ -2608,7 +2585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" s="6">
         <v>1</v>
       </c>
@@ -2620,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" s="6">
         <v>1</v>
       </c>
@@ -2632,7 +2609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" s="6">
         <v>1</v>
       </c>
@@ -2644,7 +2621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" s="6">
         <v>1</v>
       </c>
@@ -2656,7 +2633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" s="6">
         <v>1</v>
       </c>
@@ -2668,7 +2645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" s="6">
         <v>1</v>
       </c>
@@ -2680,7 +2657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" s="6">
         <v>1</v>
       </c>
@@ -2692,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" s="6">
         <v>1</v>
       </c>
@@ -2704,7 +2681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" s="6">
         <v>1</v>
       </c>
@@ -2716,7 +2693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" s="6">
         <v>1</v>
       </c>
@@ -2729,7 +2706,7 @@
         <v>94.7</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" s="6">
         <v>1</v>
       </c>
@@ -2741,7 +2718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" s="6">
         <v>1</v>
       </c>
@@ -2753,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" s="6">
         <v>1</v>
       </c>
@@ -2765,7 +2742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" s="6">
         <v>1</v>
       </c>
@@ -2777,7 +2754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" s="6">
         <v>1</v>
       </c>
@@ -2789,7 +2766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" s="6">
         <v>1</v>
       </c>
@@ -2801,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" s="6">
         <v>1</v>
       </c>
@@ -2813,7 +2790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" s="6">
         <v>1</v>
       </c>
@@ -2825,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" s="6">
         <v>1</v>
       </c>
@@ -2837,7 +2814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" s="6">
         <v>1</v>
       </c>
@@ -2849,7 +2826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" s="6">
         <v>1</v>
       </c>
@@ -2861,7 +2838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" s="6">
         <v>1</v>
       </c>
@@ -2873,7 +2850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194" s="6">
         <v>1</v>
       </c>
@@ -2885,7 +2862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195" s="6">
         <v>1</v>
       </c>
@@ -2897,7 +2874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196" s="6">
         <v>1</v>
       </c>
@@ -2909,7 +2886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197" s="6">
         <v>1</v>
       </c>
@@ -2921,7 +2898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198" s="6">
         <v>1</v>
       </c>
@@ -2933,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199" s="6">
         <v>1</v>
       </c>
@@ -2945,7 +2922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200" s="6">
         <v>1</v>
       </c>
@@ -2957,7 +2934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201" s="6">
         <v>1</v>
       </c>
@@ -2969,7 +2946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202" s="6">
         <v>1</v>
       </c>
@@ -2981,7 +2958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A203" s="6">
         <v>1</v>
       </c>
@@ -2993,7 +2970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204" s="6">
         <v>1</v>
       </c>
@@ -3005,7 +2982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A205" s="6">
         <v>1</v>
       </c>
@@ -3017,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A206" s="6">
         <v>1</v>
       </c>
@@ -3029,7 +3006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A207" s="6">
         <v>1</v>
       </c>
@@ -3041,7 +3018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A208" s="6">
         <v>1</v>
       </c>
@@ -3053,7 +3030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A209" s="6">
         <v>1</v>
       </c>
@@ -3065,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A210" s="6">
         <v>1</v>
       </c>
@@ -3077,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A211" s="6">
         <v>1</v>
       </c>
@@ -3089,7 +3066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A212" s="6">
         <v>1</v>
       </c>
@@ -3101,7 +3078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A213" s="6">
         <v>1</v>
       </c>
@@ -3113,7 +3090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A214" s="6">
         <v>1</v>
       </c>
@@ -3125,7 +3102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A215" s="6">
         <v>1</v>
       </c>
@@ -3137,7 +3114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A216" s="6">
         <v>1</v>
       </c>
@@ -3149,7 +3126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A217" s="6">
         <v>1</v>
       </c>
@@ -3161,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A218" s="6">
         <v>1</v>
       </c>
@@ -3173,7 +3150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A219" s="6">
         <v>1</v>
       </c>
@@ -3185,7 +3162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A220" s="6">
         <v>1</v>
       </c>
@@ -3197,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A221" s="6">
         <v>1</v>
       </c>
@@ -3209,7 +3186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A222" s="6">
         <v>1</v>
       </c>
@@ -3221,7 +3198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A223" s="6">
         <v>1</v>
       </c>
@@ -3233,7 +3210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A224" s="6">
         <v>1</v>
       </c>
@@ -3245,7 +3222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A225" s="6">
         <v>1</v>
       </c>
@@ -3257,7 +3234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A226" s="6">
         <v>1</v>
       </c>
@@ -3269,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A227" s="6">
         <v>1</v>
       </c>
@@ -3281,7 +3258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A228" s="6">
         <v>1</v>
       </c>
@@ -3293,7 +3270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A229" s="6">
         <v>1</v>
       </c>
@@ -3305,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A230" s="6">
         <v>1</v>
       </c>
@@ -3317,7 +3294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A231" s="6">
         <v>1</v>
       </c>
@@ -3329,7 +3306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A232" s="6">
         <v>1</v>
       </c>
@@ -3341,7 +3318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A233" s="6">
         <v>1</v>
       </c>
@@ -3353,7 +3330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A234" s="6">
         <v>1</v>
       </c>
@@ -3365,7 +3342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A235" s="6">
         <v>1</v>
       </c>
@@ -3377,7 +3354,7 @@
         <v>50.2</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A236" s="6">
         <v>1</v>
       </c>
@@ -3389,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A237" s="6">
         <v>1</v>
       </c>
@@ -3401,7 +3378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A238" s="6">
         <v>1</v>
       </c>
@@ -3413,7 +3390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239" s="6">
         <v>1</v>
       </c>
@@ -3425,7 +3402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240" s="6">
         <v>1</v>
       </c>
@@ -3437,7 +3414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241" s="6">
         <v>1</v>
       </c>
@@ -3449,7 +3426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242" s="6">
         <v>1</v>
       </c>
@@ -3461,7 +3438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243" s="6">
         <v>1</v>
       </c>
@@ -3473,7 +3450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A244" s="6">
         <v>1</v>
       </c>
@@ -3485,7 +3462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A245" s="6">
         <v>1</v>
       </c>
@@ -3497,7 +3474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A246" s="6">
         <v>1</v>
       </c>
@@ -3509,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A247" s="6">
         <v>1</v>
       </c>
@@ -3521,7 +3498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A248" s="6">
         <v>1</v>
       </c>
@@ -3533,7 +3510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A249" s="6">
         <v>1</v>
       </c>
@@ -3545,7 +3522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A250" s="6">
         <v>1</v>
       </c>
@@ -3557,7 +3534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A251" s="6">
         <v>1</v>
       </c>
@@ -3569,7 +3546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A252" s="6">
         <v>1</v>
       </c>
@@ -3581,7 +3558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A253" s="6">
         <v>1</v>
       </c>
@@ -3593,7 +3570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A254" s="6">
         <v>1</v>
       </c>
@@ -3605,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A255" s="6">
         <v>1</v>
       </c>
@@ -3617,7 +3594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A256" s="6">
         <v>1</v>
       </c>
@@ -3629,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A257" s="6">
         <v>1</v>
       </c>
@@ -3641,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A258" s="6">
         <v>1</v>
       </c>
@@ -3653,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A259" s="6">
         <v>1</v>
       </c>
@@ -3665,7 +3642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A260" s="6">
         <v>1</v>
       </c>
@@ -3677,7 +3654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A261" s="6">
         <v>1</v>
       </c>
@@ -3689,7 +3666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A262" s="6">
         <v>1</v>
       </c>
@@ -3701,7 +3678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A263" s="6">
         <v>1</v>
       </c>
@@ -3713,7 +3690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A264" s="6">
         <v>1</v>
       </c>
@@ -3725,7 +3702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A265" s="6">
         <v>1</v>
       </c>
@@ -3737,7 +3714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A266" s="6">
         <v>1</v>
       </c>
@@ -3749,7 +3726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A267" s="6">
         <v>1</v>
       </c>
@@ -3761,7 +3738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A268" s="6">
         <v>1</v>
       </c>
@@ -3773,7 +3750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A269" s="6">
         <v>1</v>
       </c>
@@ -3785,7 +3762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A270" s="6">
         <v>1</v>
       </c>
@@ -3797,7 +3774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A271" s="6">
         <v>1</v>
       </c>
@@ -3809,7 +3786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A272" s="6">
         <v>1</v>
       </c>
@@ -3821,7 +3798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A273" s="6">
         <v>1</v>
       </c>
@@ -3833,7 +3810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A274" s="6">
         <v>1</v>
       </c>
@@ -3845,7 +3822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A275" s="6">
         <v>1</v>
       </c>
@@ -3857,7 +3834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A276" s="6">
         <v>1</v>
       </c>
@@ -3869,7 +3846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A277" s="6">
         <v>1</v>
       </c>
@@ -3881,7 +3858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A278" s="6">
         <v>1</v>
       </c>
@@ -3893,7 +3870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A279" s="6">
         <v>1</v>
       </c>
@@ -3905,7 +3882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A280" s="6">
         <v>1</v>
       </c>
@@ -3917,7 +3894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A281" s="6">
         <v>1</v>
       </c>
@@ -3929,7 +3906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A282" s="6">
         <v>1</v>
       </c>
@@ -3941,7 +3918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A283" s="6">
         <v>1</v>
       </c>
@@ -3953,7 +3930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A284" s="6">
         <v>1</v>
       </c>
@@ -3965,7 +3942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A285" s="6">
         <v>1</v>
       </c>
@@ -3977,7 +3954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A286" s="6">
         <v>1</v>
       </c>
@@ -3989,7 +3966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A287" s="6">
         <v>1</v>
       </c>
@@ -4001,7 +3978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A288" s="6">
         <v>1</v>
       </c>
@@ -4013,7 +3990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A289" s="6">
         <v>1</v>
       </c>
@@ -4025,7 +4002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A290" s="6">
         <v>1</v>
       </c>
@@ -4051,9 +4028,9 @@
       <selection activeCell="C15" sqref="C15:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>2</v>
       </c>
@@ -4068,7 +4045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -4083,7 +4060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4098,7 +4075,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4113,7 +4090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4128,7 +4105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -4143,7 +4120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -4158,7 +4135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -4173,7 +4150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -4188,7 +4165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -4203,7 +4180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -4218,7 +4195,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -4233,7 +4210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -4248,7 +4225,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -4263,7 +4240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -4278,7 +4255,7 @@
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -4293,7 +4270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -4308,7 +4285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -4323,7 +4300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -4338,7 +4315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -4353,7 +4330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -4368,7 +4345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -4385,7 +4362,7 @@
         <v>26.3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
@@ -4400,7 +4377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>2</v>
       </c>
@@ -4418,7 +4395,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
@@ -4433,7 +4410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
@@ -4448,7 +4425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
@@ -4463,7 +4440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
@@ -4478,7 +4455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>3</v>
       </c>
@@ -4493,7 +4470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -4508,7 +4485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -4523,7 +4500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -4538,7 +4515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3</v>
       </c>
@@ -4553,7 +4530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
@@ -4568,7 +4545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3</v>
       </c>
@@ -4583,7 +4560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>3</v>
       </c>
@@ -4598,7 +4575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>3</v>
       </c>
@@ -4613,7 +4590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>3</v>
       </c>
@@ -4628,7 +4605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3</v>
       </c>
@@ -4643,7 +4620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>3</v>
       </c>
@@ -4658,7 +4635,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>3</v>
       </c>
@@ -4673,7 +4650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>3</v>
       </c>
@@ -4690,7 +4667,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>3</v>
       </c>
@@ -4705,7 +4682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>3</v>
       </c>
@@ -4720,7 +4697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>3</v>
       </c>
@@ -4735,7 +4712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>3</v>
       </c>
@@ -4750,7 +4727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>3</v>
       </c>
@@ -4765,7 +4742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>3</v>
       </c>
@@ -4783,7 +4760,7 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>4</v>
       </c>
@@ -4798,7 +4775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>4</v>
       </c>
@@ -4813,7 +4790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>4</v>
       </c>
@@ -4828,7 +4805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>4</v>
       </c>
@@ -4843,7 +4820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>4</v>
       </c>
@@ -4858,7 +4835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>4</v>
       </c>
@@ -4873,7 +4850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>4</v>
       </c>
@@ -4888,7 +4865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>4</v>
       </c>
@@ -4903,7 +4880,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>4</v>
       </c>
@@ -4918,7 +4895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>4</v>
       </c>
@@ -4933,7 +4910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>4</v>
       </c>
@@ -4948,7 +4925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>4</v>
       </c>
@@ -4963,7 +4940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>4</v>
       </c>
@@ -4978,7 +4955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>4</v>
       </c>
@@ -4993,7 +4970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>4</v>
       </c>
@@ -5008,7 +4985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>4</v>
       </c>
@@ -5023,7 +5000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>4</v>
       </c>
@@ -5038,7 +5015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>4</v>
       </c>
@@ -5055,7 +5032,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>4</v>
       </c>
@@ -5070,7 +5047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>4</v>
       </c>
@@ -5085,7 +5062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>4</v>
       </c>
@@ -5100,7 +5077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>4</v>
       </c>
@@ -5115,7 +5092,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>4</v>
       </c>
@@ -5130,7 +5107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>4</v>
       </c>
@@ -5148,7 +5125,7 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>5</v>
       </c>
@@ -5163,7 +5140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>5</v>
       </c>
@@ -5178,7 +5155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>5</v>
       </c>
@@ -5193,7 +5170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>5</v>
       </c>
@@ -5208,7 +5185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>5</v>
       </c>
@@ -5223,7 +5200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>5</v>
       </c>
@@ -5238,7 +5215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>5</v>
       </c>
@@ -5253,7 +5230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>5</v>
       </c>
@@ -5268,7 +5245,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>5</v>
       </c>
@@ -5283,7 +5260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>5</v>
       </c>
@@ -5298,7 +5275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>5</v>
       </c>
@@ -5313,7 +5290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>5</v>
       </c>
@@ -5328,7 +5305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>5</v>
       </c>
@@ -5343,7 +5320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>5</v>
       </c>
@@ -5358,7 +5335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>5</v>
       </c>
@@ -5373,7 +5350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>5</v>
       </c>
@@ -5390,7 +5367,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>5</v>
       </c>
@@ -5405,7 +5382,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>5</v>
       </c>
@@ -5420,7 +5397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>5</v>
       </c>
@@ -5437,7 +5414,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>5</v>
       </c>
@@ -5452,7 +5429,7 @@
         <v>41.7</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>5</v>
       </c>
@@ -5467,7 +5444,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>5</v>
       </c>
@@ -5482,7 +5459,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>5</v>
       </c>
@@ -5497,7 +5474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>5</v>
       </c>
@@ -5515,7 +5492,7 @@
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
     </row>
-    <row r="97" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>6</v>
       </c>
@@ -5530,7 +5507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>6</v>
       </c>
@@ -5545,7 +5522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>6</v>
       </c>
@@ -5560,7 +5537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>6</v>
       </c>
@@ -5575,7 +5552,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>6</v>
       </c>
@@ -5590,7 +5567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>6</v>
       </c>
@@ -5605,7 +5582,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>6</v>
       </c>
@@ -5620,7 +5597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>6</v>
       </c>
@@ -5635,7 +5612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>6</v>
       </c>
@@ -5650,7 +5627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>6</v>
       </c>
@@ -5665,7 +5642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>6</v>
       </c>
@@ -5680,7 +5657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>6</v>
       </c>
@@ -5695,7 +5672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>6</v>
       </c>
@@ -5710,7 +5687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>6</v>
       </c>
@@ -5725,7 +5702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>6</v>
       </c>
@@ -5740,7 +5717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>6</v>
       </c>
@@ -5755,7 +5732,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>6</v>
       </c>
@@ -5770,7 +5747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>6</v>
       </c>
@@ -5785,7 +5762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>6</v>
       </c>
@@ -5800,7 +5777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>6</v>
       </c>
@@ -5815,7 +5792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>6</v>
       </c>
@@ -5830,7 +5807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>6</v>
       </c>
@@ -5845,7 +5822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>6</v>
       </c>
@@ -5860,7 +5837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>6</v>
       </c>
@@ -5878,7 +5855,7 @@
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
     </row>
-    <row r="121" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="121" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>